<commit_message>
Fixed bug in Logo Modeloramas KPI
</commit_message>
<xml_diff>
--- a/Projects/INBEVTRADMX/Data/inbevtradmx_template_3_partial_v2.xlsx
+++ b/Projects/INBEVTRADMX/Data/inbevtradmx_template_3_partial_v2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="183">
   <si>
     <t xml:space="preserve">KPI Level 1 Name</t>
   </si>
@@ -423,6 +423,9 @@
   </si>
   <si>
     <t xml:space="preserve">Hay o no hay logo?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logo Moderlorama Exterior</t>
   </si>
   <si>
     <t xml:space="preserve">At least 1 facing of "Logo Modelorama Exterior" in Scene Type "Logo Modelorama Exterior", then pass.</t>
@@ -895,17 +898,19 @@
   </sheetPr>
   <dimension ref="A1:U65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G55" activeCellId="0" sqref="G55"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R35" activeCellId="0" sqref="R35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.3877551020408"/>
-    <col collapsed="false" hidden="false" max="19" min="7" style="0" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="57.234693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="37.9234693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="41.8469387755102"/>
+    <col collapsed="false" hidden="false" max="19" min="7" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="56.5612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2902,10 +2907,10 @@
       </c>
       <c r="Q35" s="6"/>
       <c r="R35" s="6" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="S35" s="6" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="T35" s="10" t="s">
         <v>100</v>
@@ -2919,10 +2924,10 @@
         <v>90</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>23</v>
@@ -2959,10 +2964,10 @@
       </c>
       <c r="Q36" s="6"/>
       <c r="R36" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="S36" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="T36" s="10" t="s">
         <v>100</v>
@@ -2976,10 +2981,10 @@
         <v>90</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>23</v>
@@ -3016,10 +3021,10 @@
       </c>
       <c r="Q37" s="6"/>
       <c r="R37" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="S37" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="T37" s="10" t="s">
         <v>100</v>
@@ -3033,17 +3038,17 @@
         <v>90</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E38" s="6"/>
       <c r="F38" s="6" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G38" s="6" t="s">
         <v>24</v>
@@ -3075,13 +3080,13 @@
       </c>
       <c r="Q38" s="6"/>
       <c r="R38" s="6" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="S38" s="6" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="T38" s="10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U38" s="6" t="s">
         <v>32</v>
@@ -3092,17 +3097,17 @@
         <v>90</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E39" s="6"/>
       <c r="F39" s="6" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="G39" s="6" t="s">
         <v>24</v>
@@ -3134,13 +3139,13 @@
       </c>
       <c r="Q39" s="6"/>
       <c r="R39" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="S39" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="T39" s="10" t="s">
         <v>146</v>
-      </c>
-      <c r="S39" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="T39" s="10" t="s">
-        <v>145</v>
       </c>
       <c r="U39" s="6" t="s">
         <v>32</v>
@@ -3148,7 +3153,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>22</v>
@@ -3195,7 +3200,7 @@
         <v>27</v>
       </c>
       <c r="Q40" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="R40" s="8" t="s">
         <v>29</v>
@@ -3212,7 +3217,7 @@
     </row>
     <row r="41" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>46</v>
@@ -3253,7 +3258,7 @@
         <v>27</v>
       </c>
       <c r="Q41" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="R41" s="8" t="s">
         <v>29</v>
@@ -3270,7 +3275,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>56</v>
@@ -3313,7 +3318,7 @@
         <v>27</v>
       </c>
       <c r="Q42" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="R42" s="8" t="s">
         <v>24</v>
@@ -3330,7 +3335,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="8" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>70</v>
@@ -3371,7 +3376,7 @@
         <v>27</v>
       </c>
       <c r="Q43" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="R43" s="8" t="s">
         <v>29</v>
@@ -3388,7 +3393,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>22</v>
@@ -3429,7 +3434,7 @@
         <v>76</v>
       </c>
       <c r="Q44" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="R44" s="8" t="s">
         <v>77</v>
@@ -3446,7 +3451,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>78</v>
@@ -3489,7 +3494,7 @@
         <v>76</v>
       </c>
       <c r="Q45" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="R45" s="8" t="s">
         <v>24</v>
@@ -3506,7 +3511,7 @@
     </row>
     <row r="46" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>81</v>
@@ -3549,7 +3554,7 @@
         <v>76</v>
       </c>
       <c r="Q46" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="R46" s="8" t="s">
         <v>24</v>
@@ -3566,10 +3571,10 @@
     </row>
     <row r="47" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="8" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C47" s="6" t="str">
         <f aca="false">B47</f>
@@ -3609,7 +3614,7 @@
         <v>76</v>
       </c>
       <c r="Q47" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="R47" s="8" t="s">
         <v>24</v>
@@ -3629,17 +3634,17 @@
         <v>90</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E48" s="6"/>
       <c r="F48" s="6" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G48" s="6" t="s">
         <v>24</v>
@@ -3671,13 +3676,13 @@
       </c>
       <c r="Q48" s="6"/>
       <c r="R48" s="16" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="S48" s="16" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="T48" s="10" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="U48" s="6" t="s">
         <v>32</v>
@@ -3710,107 +3715,107 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="C5" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="D5" s="0" t="s">
         <v>165</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="0" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="0" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="D11" s="0" t="s">
         <v>172</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C13" s="0" t="s">
+        <v>176</v>
+      </c>
+      <c r="D13" s="0" t="s">
         <v>175</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C14" s="0" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
     </row>
   </sheetData>
@@ -3837,7 +3842,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3863,27 +3868,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -3910,12 +3915,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.1224489795918"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>